<commit_message>
Test Tomcat Connection Pooling
</commit_message>
<xml_diff>
--- a/me_docs/10.Build-A-Complete-Database-Web-App-with-JDBC.xlsx
+++ b/me_docs/10.Build-A-Complete-Database-Web-App-with-JDBC.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7477E4D2-87DE-464B-A684-72F3B7548FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D04378E-AB66-47AE-935C-BF30C6157A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sơ đồ" sheetId="1" r:id="rId1"/>
     <sheet name="Setting Project Database" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Tomcat Connection" sheetId="3" r:id="rId3"/>
+    <sheet name="MVC" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Bật Xammp</t>
   </si>
@@ -38,6 +40,27 @@
   </si>
   <si>
     <t>Run script 02-student-tracker.sql</t>
+  </si>
+  <si>
+    <t>Create web-student-tracker project</t>
+  </si>
+  <si>
+    <t>Copy mysql-connector-java-8.0.13.jar to project</t>
+  </si>
+  <si>
+    <t>Copy context.xml to Project</t>
+  </si>
+  <si>
+    <t>Create com.luv2code.web.jdbc package</t>
+  </si>
+  <si>
+    <t>Create TestServlet</t>
+  </si>
+  <si>
+    <t>Run Server</t>
+  </si>
+  <si>
+    <t>Access URL: http://localhost:8080/web-student-tracker/TestServlet</t>
   </si>
 </sst>
 </file>
@@ -487,6 +510,984 @@
         <a:xfrm>
           <a:off x="609600" y="33718500"/>
           <a:ext cx="6457143" cy="3666667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>8762</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>151762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B39A171-7D55-4730-9A59-2C57F875C75B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6104762" cy="5104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>456457</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>122976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6AE6A64-04B6-4EE0-A39A-6F76721F0B10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="5942857" cy="6790476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>332876</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>113738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C706964E-9BBF-4E9D-9174-5B903C608C94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="12954000"/>
+          <a:ext cx="3990476" cy="4495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>37257</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>8881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95A415F4-53F9-4D77-8FF1-83176F3284C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="23241000"/>
+          <a:ext cx="6742857" cy="5152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>66167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{875E0F7B-C258-4635-AA7A-1279858A1A90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="28575000"/>
+          <a:ext cx="4876190" cy="4066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>37714</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>180548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F46047F3-0B73-456D-96D6-892561319272}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="32766000"/>
+          <a:ext cx="3085714" cy="3419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>475429</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>18405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C5CA722-9AFA-434F-96D1-84136F954D19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="36576000"/>
+          <a:ext cx="6571429" cy="5161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>238</xdr:row>
+      <xdr:rowOff>161476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3BB2BF0-F44D-4669-AEEB-21C8A6C3BD64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="41910000"/>
+          <a:ext cx="4866667" cy="3590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>66095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{505DC555-7C33-48BC-A40F-24F2E3613F8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="45720000"/>
+          <a:ext cx="4866667" cy="4638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>266</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>113714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3463DCA8-E434-461E-BF12-D408800D2970}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="50673000"/>
+          <a:ext cx="4866667" cy="4685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>319</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>605530</xdr:colOff>
+      <xdr:row>369</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A1F29E4-E036-4C9F-A7C5-3143EB570434}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609599" y="60959999"/>
+          <a:ext cx="7920731" cy="9363076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>319</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>17600</xdr:colOff>
+      <xdr:row>346</xdr:row>
+      <xdr:rowOff>46976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38B600C8-9DFF-4893-B1D4-3027A48AE11D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="60769500"/>
+          <a:ext cx="11600000" cy="5190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>347</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>532724</xdr:colOff>
+      <xdr:row>368</xdr:row>
+      <xdr:rowOff>104262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29545937-1CF4-414A-B943-B950BD3FEBF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="66103500"/>
+          <a:ext cx="5409524" cy="4104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>370</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>199086</xdr:colOff>
+      <xdr:row>398</xdr:row>
+      <xdr:rowOff>75524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD89AA7B-FB94-4DD9-8CD1-BCE38546E433}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="70485000"/>
+          <a:ext cx="7514286" cy="5409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>401</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523048</xdr:colOff>
+      <xdr:row>428</xdr:row>
+      <xdr:rowOff>18405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA71B91F-A107-4FB1-A94F-D17553A4B4AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="76390500"/>
+          <a:ext cx="6619048" cy="5161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>429</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>294629</xdr:colOff>
+      <xdr:row>462</xdr:row>
+      <xdr:rowOff>142071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDC1F7E3-E0BE-4DC3-BEEB-0FF09567C50D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="81724500"/>
+          <a:ext cx="5171429" cy="6428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>608584</xdr:colOff>
+      <xdr:row>318</xdr:row>
+      <xdr:rowOff>47031</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E85B824-0DE8-40F6-A4A0-1FF0022715C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8943975" y="55873650"/>
+          <a:ext cx="8123809" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>292</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>37105</xdr:colOff>
+      <xdr:row>319</xdr:row>
+      <xdr:rowOff>8881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24B1E9FF-7C3A-443F-8F7A-E1D64FD25D43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="55626000"/>
+          <a:ext cx="7961905" cy="5152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>455848</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>27976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4B3C0F4-3248-4588-83F7-1F772F7CA91D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="17907000"/>
+          <a:ext cx="10819048" cy="4790476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>465</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47009</xdr:colOff>
+      <xdr:row>474</xdr:row>
+      <xdr:rowOff>47405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9921313-ABA1-4964-98AD-575DD60B0558}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="88582500"/>
+          <a:ext cx="4923809" cy="1761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>465</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>237333</xdr:colOff>
+      <xdr:row>482</xdr:row>
+      <xdr:rowOff>66262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C7FCBE8-3749-401D-96D1-D1EB9AD97E8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="88582500"/>
+          <a:ext cx="6333333" cy="3304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>122362</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{109FD6E0-4A9A-4092-A919-C67E413081F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="190500"/>
+          <a:ext cx="11704762" cy="4695238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -778,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{933FDFA9-9F5E-4EAF-93EE-D3E486942C99}">
   <dimension ref="A2:B149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="B199" sqref="B199"/>
+    <sheetView topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="P187" sqref="P187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,4 +1809,70 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45B62C4-479A-4E01-9699-9D7115484A7B}">
+  <dimension ref="A2:A465"/>
+  <sheetViews>
+    <sheetView topLeftCell="A465" workbookViewId="0">
+      <selection activeCell="D485" sqref="D484:D485"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F163C1AA-9C6A-4BD7-BA3B-BFD847D8F60D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
List Students - Creating the JDBC Code
</commit_message>
<xml_diff>
--- a/me_docs/10.Build-A-Complete-Database-Web-App-with-JDBC.xlsx
+++ b/me_docs/10.Build-A-Complete-Database-Web-App-with-JDBC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55379344-A26C-47E9-B1BA-F39AC5D99322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599A8D7D-5962-499C-98B3-DA773CD2B562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sơ đồ" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Test Tomcat Connection" sheetId="3" r:id="rId3"/>
     <sheet name="MVC" sheetId="4" r:id="rId4"/>
     <sheet name="Create Student class" sheetId="5" r:id="rId5"/>
+    <sheet name="List Students" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Bật Xammp</t>
   </si>
@@ -77,6 +78,15 @@
   </si>
   <si>
     <t>Add toString method</t>
+  </si>
+  <si>
+    <t>Create StudentDbUtil class</t>
+  </si>
+  <si>
+    <t>getStudents method</t>
+  </si>
+  <si>
+    <t>close method</t>
   </si>
 </sst>
 </file>
@@ -2169,6 +2179,363 @@
         <a:xfrm>
           <a:off x="609600" y="77343000"/>
           <a:ext cx="8390476" cy="4342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>218209</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A41ED965-6D7C-42F4-8AF3-632CD8527D6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6923809" cy="5076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>132724</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>123071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7E6C0F9-6B86-4F8D-9E57-BF2631381D0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="5009524" cy="6028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>580038</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>132857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59BA32EB-BDE3-467B-BEC6-EF47CB173EDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11811000"/>
+          <a:ext cx="7895238" cy="3942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>583058</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDF6BC0-930F-47D6-A6C7-569506BF0B31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16002001"/>
+          <a:ext cx="7898258" cy="9258300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>37181</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>75571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9756CD18-72DF-465A-A7FC-9481D27E7567}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="16002000"/>
+          <a:ext cx="7352381" cy="5028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>504152</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>94738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30449E01-91BD-4131-B40E-71AFFEBB32D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="21145500"/>
+          <a:ext cx="5380952" cy="4095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>484648</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>151643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0010884-19C4-4FBD-9711-CEBC516235E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="25527000"/>
+          <a:ext cx="9019048" cy="6057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>170590</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>171095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA6B92B0-FC3A-46AF-A575-81190969242F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="32194500"/>
+          <a:ext cx="6876190" cy="2838095"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2496,7 +2863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45B62C4-479A-4E01-9699-9D7115484A7B}">
   <dimension ref="A2:A465"/>
   <sheetViews>
-    <sheetView topLeftCell="A465" workbookViewId="0">
+    <sheetView topLeftCell="A337" workbookViewId="0">
       <selection activeCell="D485" sqref="D484:D485"/>
     </sheetView>
   </sheetViews>
@@ -2547,7 +2914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F163C1AA-9C6A-4BD7-BA3B-BFD847D8F60D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -2562,7 +2929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537638A7-42CF-4CF6-A718-9E5CFB98E201}">
   <dimension ref="A2:A346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
+    <sheetView topLeftCell="A410" workbookViewId="0">
       <selection activeCell="B431" sqref="B431"/>
     </sheetView>
   </sheetViews>
@@ -2597,4 +2964,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7457EF-1F6F-4721-8B25-E1D036CFBADA}">
+  <dimension ref="A2:A170"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="G193" sqref="G193"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
List Students - Building the Servlet
</commit_message>
<xml_diff>
--- a/me_docs/10.Build-A-Complete-Database-Web-App-with-JDBC.xlsx
+++ b/me_docs/10.Build-A-Complete-Database-Web-App-with-JDBC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599A8D7D-5962-499C-98B3-DA773CD2B562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84078C9D-4ED8-4A60-90D2-FBF8E589CD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sơ đồ" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Test Tomcat Connection" sheetId="3" r:id="rId3"/>
     <sheet name="MVC" sheetId="4" r:id="rId4"/>
     <sheet name="Create Student class" sheetId="5" r:id="rId5"/>
-    <sheet name="List Students" sheetId="6" r:id="rId6"/>
+    <sheet name="StudentDbUtil Class" sheetId="6" r:id="rId6"/>
+    <sheet name="StudentControllerServlet Class" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Bật Xammp</t>
   </si>
@@ -88,6 +89,18 @@
   <si>
     <t>close method</t>
   </si>
+  <si>
+    <t>Create StudentControllerServlet class</t>
+  </si>
+  <si>
+    <t>Initialize studentDbUtil</t>
+  </si>
+  <si>
+    <t>doGet method</t>
+  </si>
+  <si>
+    <t>listStudents method</t>
+  </si>
 </sst>
 </file>
 
@@ -2536,6 +2549,583 @@
         <a:xfrm>
           <a:off x="609600" y="32194500"/>
           <a:ext cx="6876190" cy="2838095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>208686</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>151762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09D1C132-5B2D-4B93-894A-FB67B1821C75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6914286" cy="5104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>589943</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>151952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37EC3B05-51DC-4731-9BE9-CCA43CDF7E8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="4857143" cy="3580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>66095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A1D8F06-60B1-4775-AF79-209DDDD161AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9525000"/>
+          <a:ext cx="4876190" cy="4638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8914</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>47048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DDD6D9F-8534-4578-AE80-B1377D512DF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="14287500"/>
+          <a:ext cx="4885714" cy="4619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>580038</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>46976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB5B177-69F2-441D-BA33-DB8088C15D66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="19050000"/>
+          <a:ext cx="7895238" cy="5190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>27124</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>27929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB6BB550-9E40-4E6E-8658-0E9A5AA3AB7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="24765000"/>
+          <a:ext cx="11609524" cy="5171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561371</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>85048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78C88EF-E4B6-4C04-8094-19076BFE78B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="30099000"/>
+          <a:ext cx="4828571" cy="5419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>65219</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>37357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2834BDFB-DBD8-4138-A3B4-A5FA0D33C889}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="35623500"/>
+          <a:ext cx="11647619" cy="5942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>221</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>8076</xdr:colOff>
+      <xdr:row>248</xdr:row>
+      <xdr:rowOff>46976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6546F67E-AE8F-47EC-9256-065B3191897D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="42100500"/>
+          <a:ext cx="11590476" cy="5190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>598628</xdr:colOff>
+      <xdr:row>278</xdr:row>
+      <xdr:rowOff>18405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDF5E409-9D0A-4E2A-8CA0-994AFBB2249D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="47815500"/>
+          <a:ext cx="11571428" cy="5161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>279</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>579581</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>18405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FC48FAA-D5D7-45B7-8D1B-83D09271D37F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="53149500"/>
+          <a:ext cx="11552381" cy="5161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>307</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>17600</xdr:colOff>
+      <xdr:row>334</xdr:row>
+      <xdr:rowOff>18405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D654A0F0-91B6-4562-9978-DF61256A097E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="58483500"/>
+          <a:ext cx="11600000" cy="5161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>335</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>55695</xdr:colOff>
+      <xdr:row>363</xdr:row>
+      <xdr:rowOff>8857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFF5AB90-1AE1-4722-877F-1832104888DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="63817500"/>
+          <a:ext cx="11638095" cy="5342857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2970,7 +3560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7457EF-1F6F-4721-8B25-E1D036CFBADA}">
   <dimension ref="A2:A170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="G193" sqref="G193"/>
     </sheetView>
   </sheetViews>
@@ -2995,4 +3585,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADB2A70-F898-4357-8581-2CA69E6CD933}">
+  <dimension ref="A2:A251"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="B365" sqref="B365"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
List Students - Developing the JSP
</commit_message>
<xml_diff>
--- a/me_docs/10.Build-A-Complete-Database-Web-App-with-JDBC.xlsx
+++ b/me_docs/10.Build-A-Complete-Database-Web-App-with-JDBC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84078C9D-4ED8-4A60-90D2-FBF8E589CD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A59FCAE-EE0E-4073-93D8-33D43D73D524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sơ đồ" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Create Student class" sheetId="5" r:id="rId5"/>
     <sheet name="StudentDbUtil Class" sheetId="6" r:id="rId6"/>
     <sheet name="StudentControllerServlet Class" sheetId="7" r:id="rId7"/>
+    <sheet name="Developing the JSP" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Bật Xammp</t>
   </si>
@@ -101,6 +102,21 @@
   <si>
     <t>listStudents method</t>
   </si>
+  <si>
+    <t>Create list-students.jsp</t>
+  </si>
+  <si>
+    <t>javax.servlet.jsp.jstl-1.2.1.jar</t>
+  </si>
+  <si>
+    <t>javax.servlet.jsp.jstl-api-1.2.1.jar</t>
+  </si>
+  <si>
+    <t>Copy and paste jar file</t>
+  </si>
+  <si>
+    <t>Access browser to test http://localhost:8080/web-student-tracker/StudentControllerServlet</t>
+  </si>
 </sst>
 </file>
 
@@ -3126,6 +3142,231 @@
         <a:xfrm>
           <a:off x="609600" y="63817500"/>
           <a:ext cx="11638095" cy="5342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>37257</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>56500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45F864B8-8A59-49E8-A383-801C417E6310}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6742857" cy="5200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>170738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6346E29D-C18B-418E-88AF-B57BBC7C289B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="4866667" cy="5695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>113905</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161309</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB59F72-D2A8-4EFD-AA29-0F29D6110E10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="3161905" cy="4923809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>313143</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>94500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97C93EA6-6793-446F-9DF7-5A3AD41D46F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="17335500"/>
+          <a:ext cx="9457143" cy="6000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161219</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>18714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68EE103C-55C4-4D44-89C8-8E55262A757C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="23812500"/>
+          <a:ext cx="5647619" cy="2685714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3591,7 +3832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADB2A70-F898-4357-8581-2CA69E6CD933}">
   <dimension ref="A2:A251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+    <sheetView topLeftCell="A340" workbookViewId="0">
       <selection activeCell="B365" sqref="B365"/>
     </sheetView>
   </sheetViews>
@@ -3621,4 +3862,45 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F249F7-1F6E-41E4-AEBD-922257757F28}">
+  <dimension ref="A2:B125"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>